<commit_message>
added Activation link util
</commit_message>
<xml_diff>
--- a/inputdata/TestCases.xlsx
+++ b/inputdata/TestCases.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="130">
   <si>
     <t>Run</t>
   </si>
@@ -112,130 +112,319 @@
     <t>Test Steps</t>
   </si>
   <si>
-    <t>URL=http://xcelerator.ninja
+    <t>Check Test Exists or not</t>
+  </si>
+  <si>
+    <t>tagName</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>Join as a Student</t>
+  </si>
+  <si>
+    <t>Join as a Mentor</t>
+  </si>
+  <si>
+    <t>linkText</t>
+  </si>
+  <si>
+    <t>click on login page</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>babu</t>
+  </si>
+  <si>
+    <t>clearText</t>
+  </si>
+  <si>
+    <t>Enter a valid email id</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>className</t>
+  </si>
+  <si>
+    <t>cssSelector</t>
+  </si>
+  <si>
+    <t>error-message</t>
+  </si>
+  <si>
+    <t>login_01</t>
+  </si>
+  <si>
+    <t>Locators</t>
+  </si>
+  <si>
+    <t>partialLinkText</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>login_02</t>
+  </si>
+  <si>
+    <t>find Text in the Welcome page</t>
+  </si>
+  <si>
+    <t>login page validation</t>
+  </si>
+  <si>
+    <t>refreshPage</t>
+  </si>
+  <si>
+    <t>login_03</t>
+  </si>
+  <si>
+    <t>Refresh the page</t>
+  </si>
+  <si>
+    <t>clear  Email test</t>
+  </si>
+  <si>
+    <t>Set the email text</t>
+  </si>
+  <si>
+    <t>set Password</t>
+  </si>
+  <si>
+    <t>clear password text</t>
+  </si>
+  <si>
+    <t>check Error message</t>
+  </si>
+  <si>
+    <t>Check Email Error message</t>
+  </si>
+  <si>
+    <t>check Login page can be opened</t>
+  </si>
+  <si>
+    <t>Check Error message when invalid username</t>
+  </si>
+  <si>
+    <t>check Error message when invaild Password</t>
+  </si>
+  <si>
+    <t>in milli sec</t>
+  </si>
+  <si>
+    <t>LOGIN</t>
+  </si>
+  <si>
+    <t>Password is cannot be empty</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>loginAsStudent</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>login with student</t>
+  </si>
+  <si>
+    <t>click on student</t>
+  </si>
+  <si>
+    <t>//span[text()=' Student']</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>jangir</t>
+  </si>
+  <si>
+    <t>dateOfBirth</t>
+  </si>
+  <si>
+    <t>01/01/2000</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>Chinki@123</t>
+  </si>
+  <si>
+    <t>confirmPassword</t>
+  </si>
+  <si>
+    <t>TS_005</t>
+  </si>
+  <si>
+    <t>TS_006</t>
+  </si>
+  <si>
+    <t>TS_007</t>
+  </si>
+  <si>
+    <t>TS_008</t>
+  </si>
+  <si>
+    <t>TS_009</t>
+  </si>
+  <si>
+    <t>bio</t>
+  </si>
+  <si>
+    <t>Bachelor of Engineering</t>
+  </si>
+  <si>
+    <t>Mechanical Engineering</t>
+  </si>
+  <si>
+    <t>input-group-addon</t>
+  </si>
+  <si>
+    <t>TS_010</t>
+  </si>
+  <si>
+    <t>TS_011</t>
+  </si>
+  <si>
+    <t>TS_012</t>
+  </si>
+  <si>
+    <t>TS_013</t>
+  </si>
+  <si>
+    <t>TS_014</t>
+  </si>
+  <si>
+    <t>TS_015</t>
+  </si>
+  <si>
+    <t>getActivationLinkFromMail</t>
+  </si>
+  <si>
+    <t>donotreply@xceler.ninja</t>
+  </si>
+  <si>
+    <t>activateLink</t>
+  </si>
+  <si>
+    <t>activate</t>
+  </si>
+  <si>
+    <t>URL=http://xceler.herokuapp.com/#/home
 Type=Chrome
 driverpath=D:/mydrivers/chromedriver.exe</t>
   </si>
   <si>
-    <t>Check Test Exists or not</t>
-  </si>
-  <si>
-    <t>tagName</t>
-  </si>
-  <si>
-    <t>body</t>
-  </si>
-  <si>
-    <t>Join as a Student</t>
-  </si>
-  <si>
-    <t>Join as a Mentor</t>
-  </si>
-  <si>
-    <t>linkText</t>
-  </si>
-  <si>
-    <t>click on login page</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>babu</t>
-  </si>
-  <si>
-    <t>clearText</t>
-  </si>
-  <si>
-    <t>Enter a valid email id</t>
-  </si>
-  <si>
-    <t>xpath</t>
-  </si>
-  <si>
-    <t>className</t>
-  </si>
-  <si>
-    <t>cssSelector</t>
-  </si>
-  <si>
-    <t>error-message</t>
-  </si>
-  <si>
-    <t>login_01</t>
-  </si>
-  <si>
-    <t>Locators</t>
-  </si>
-  <si>
-    <t>partialLinkText</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>Actions</t>
-  </si>
-  <si>
-    <t>login_02</t>
-  </si>
-  <si>
-    <t>find Text in the Welcome page</t>
-  </si>
-  <si>
-    <t>login page validation</t>
-  </si>
-  <si>
-    <t>refreshPage</t>
-  </si>
-  <si>
-    <t>login_03</t>
-  </si>
-  <si>
-    <t>Refresh the page</t>
-  </si>
-  <si>
-    <t>clear  Email test</t>
-  </si>
-  <si>
-    <t>Set the email text</t>
-  </si>
-  <si>
-    <t>set Password</t>
-  </si>
-  <si>
-    <t>clear password text</t>
-  </si>
-  <si>
-    <t>check Error message</t>
-  </si>
-  <si>
-    <t>Check Email Error message</t>
-  </si>
-  <si>
-    <t>check Login page can be opened</t>
-  </si>
-  <si>
-    <t>Check Error message when invalid username</t>
-  </si>
-  <si>
-    <t>check Error message when invaild Password</t>
-  </si>
-  <si>
-    <t>in milli sec</t>
-  </si>
-  <si>
-    <t>LOGIN</t>
-  </si>
-  <si>
-    <t>Password cannot be empty</t>
+    <t>deleteMail</t>
+  </si>
+  <si>
+    <t>xceler.ninja@gmail.com</t>
+  </si>
+  <si>
+    <t>delete Existing Verifcation code</t>
+  </si>
+  <si>
+    <t>TS_016</t>
+  </si>
+  <si>
+    <t>TS_017</t>
+  </si>
+  <si>
+    <t>TS_018</t>
+  </si>
+  <si>
+    <t>TS_019</t>
+  </si>
+  <si>
+    <t>//button[text()='Create Account']</t>
+  </si>
+  <si>
+    <t>This is my bio</t>
+  </si>
+  <si>
+    <t>TS_020</t>
+  </si>
+  <si>
+    <t>//button[text()='Login']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">login </t>
+  </si>
+  <si>
+    <t xml:space="preserve">After login </t>
+  </si>
+  <si>
+    <t>TS_021</t>
+  </si>
+  <si>
+    <t>TS_022</t>
+  </si>
+  <si>
+    <t>//span[text()='Name of your College ']</t>
+  </si>
+  <si>
+    <t>//span[text()='Degree ']</t>
+  </si>
+  <si>
+    <t>//span[text()='Specialization ']</t>
+  </si>
+  <si>
+    <t>//span[text()='Topics of interest']</t>
+  </si>
+  <si>
+    <t>selectFromDropBox</t>
+  </si>
+  <si>
+    <t>CTAE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical </t>
+  </si>
+  <si>
+    <t>deleteRecordFromDB</t>
+  </si>
+  <si>
+    <t>TS_023</t>
+  </si>
+  <si>
+    <t>TS_024</t>
+  </si>
+  <si>
+    <t>closeBrowser</t>
+  </si>
+  <si>
+    <t>TS_025</t>
+  </si>
+  <si>
+    <t>TS_026</t>
+  </si>
+  <si>
+    <t>TS_027</t>
+  </si>
+  <si>
+    <t>Favorite Channelss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +447,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -272,7 +469,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -323,16 +520,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -363,9 +585,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -645,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,8 +931,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -703,7 +947,7 @@
         <v>17</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>1</v>
@@ -717,19 +961,19 @@
         <v>18</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>1</v>
@@ -737,151 +981,149 @@
     </row>
     <row r="4" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="F4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>33</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G4" s="9"/>
       <c r="H4" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="H5" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>65</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G6" s="9"/>
       <c r="H6" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="H7" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>39</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>1</v>
@@ -889,47 +1131,47 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+        <v>21</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="F10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>53</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>8</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="8" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>1</v>
@@ -937,13 +1179,13 @@
     </row>
     <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>7</v>
@@ -952,55 +1194,753 @@
         <v>8</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="H12" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="C14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H13" s="8" t="s">
+      <c r="G14" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="9">
+        <v>8050827560</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="15"/>
+      <c r="H31" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" s="15"/>
+      <c r="H32" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="15">
+        <v>1000</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="15">
+        <v>2000</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" s="15"/>
+      <c r="H38" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" s="15">
+        <v>2000</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G41" s="11"/>
+      <c r="H41" s="8" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G22" r:id="rId1"/>
+    <hyperlink ref="G23" r:id="rId2"/>
+    <hyperlink ref="G24" r:id="rId3"/>
+    <hyperlink ref="G34" r:id="rId4"/>
+    <hyperlink ref="G16" r:id="rId5"/>
+    <hyperlink ref="G36" r:id="rId6"/>
+    <hyperlink ref="G37" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId8"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>KeyWord!$D$2:$D$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>F18:F41 F2:F15</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>KeyWord!$B$2:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D13</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>KeyWord!$D$2:$D$18</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F13</xm:sqref>
+          <xm:sqref>D35:D41 D16:D33 D3:D14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1013,7 +1953,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1039,10 +1979,10 @@
         <v>25</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1050,54 +1990,60 @@
         <v>26</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-    </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -1121,28 +2067,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E9"/>
+  <dimension ref="B1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -1150,7 +2097,7 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -1158,7 +2105,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1169,12 +2116,12 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -1182,7 +2129,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -1190,21 +2137,41 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D12" s="18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>